<commit_message>
Output - 2 tabs
Table mapping to MITRE ATT&CK
and Data analysis
Need to fix the table to look better.
</commit_message>
<xml_diff>
--- a/Mapping_Res_to_MitreAttack.xlsx
+++ b/Mapping_Res_to_MitreAttack.xlsx
@@ -650,7 +650,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -658,13 +658,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -679,8 +692,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1032,13 +1046,13 @@
       <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F2" t="s">
@@ -1047,22 +1061,22 @@
       <c r="G2" t="s">
         <v>67</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>31</v>
       </c>
       <c r="K2" t="s">
         <v>153</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="1" t="s">
         <v>187</v>
       </c>
       <c r="N2" t="s">
@@ -1079,34 +1093,34 @@
       <c r="C3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>68</v>
       </c>
       <c r="H3" t="s">
         <v>105</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="1" t="s">
         <v>188</v>
       </c>
       <c r="N3" t="s">
@@ -1120,7 +1134,7 @@
       <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D4" t="s">
@@ -1132,25 +1146,25 @@
       <c r="F4" t="s">
         <v>49</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="1" t="s">
         <v>121</v>
       </c>
       <c r="J4" t="s">
         <v>146</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="1" t="s">
         <v>155</v>
       </c>
       <c r="L4" t="s">
         <v>171</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="1" t="s">
         <v>189</v>
       </c>
       <c r="N4" t="s">
@@ -1170,10 +1184,10 @@
       <c r="D5" t="s">
         <v>33</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G5" t="s">
@@ -1191,10 +1205,10 @@
       <c r="K5" t="s">
         <v>156</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="1" t="s">
         <v>190</v>
       </c>
       <c r="N5" t="s">
@@ -1211,10 +1225,10 @@
       <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>51</v>
       </c>
       <c r="F6" t="s">
@@ -1232,13 +1246,13 @@
       <c r="J6" t="s">
         <v>148</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="1" t="s">
         <v>191</v>
       </c>
       <c r="N6" t="s">
@@ -1255,7 +1269,7 @@
       <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E7" t="s">
@@ -1267,13 +1281,13 @@
       <c r="G7" t="s">
         <v>33</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="1" t="s">
         <v>109</v>
       </c>
       <c r="I7" t="s">
         <v>124</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="1" t="s">
         <v>149</v>
       </c>
       <c r="K7" t="s">
@@ -1302,13 +1316,13 @@
       <c r="D8" t="s">
         <v>36</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>53</v>
       </c>
       <c r="F8" t="s">
         <v>70</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>76</v>
       </c>
       <c r="H8" t="s">
@@ -1340,7 +1354,7 @@
       <c r="C9" t="s">
         <v>27</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E9" t="s">
@@ -1358,16 +1372,16 @@
       <c r="I9" t="s">
         <v>126</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="1" t="s">
         <v>150</v>
       </c>
       <c r="K9" t="s">
         <v>160</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="1" t="s">
         <v>194</v>
       </c>
       <c r="N9" t="s">
@@ -1378,16 +1392,16 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E10" t="s">
         <v>55</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>71</v>
       </c>
       <c r="G10" t="s">
@@ -1396,16 +1410,16 @@
       <c r="H10" t="s">
         <v>111</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="1" t="s">
         <v>177</v>
       </c>
       <c r="M10" t="s">
@@ -1419,28 +1433,28 @@
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F11" t="s">
         <v>56</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="1" t="s">
         <v>162</v>
       </c>
       <c r="L11" t="s">
@@ -1451,13 +1465,13 @@
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E12" t="s">
         <v>56</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G12" t="s">
@@ -1466,7 +1480,7 @@
       <c r="H12" t="s">
         <v>113</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="1" t="s">
         <v>129</v>
       </c>
       <c r="J12" t="s">
@@ -1475,7 +1489,7 @@
       <c r="K12" t="s">
         <v>163</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="1" t="s">
         <v>179</v>
       </c>
       <c r="N12" t="s">
@@ -1483,13 +1497,13 @@
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E13" t="s">
         <v>57</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="1" t="s">
         <v>72</v>
       </c>
       <c r="G13" t="s">
@@ -1501,10 +1515,10 @@
       <c r="I13" t="s">
         <v>111</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="1" t="s">
         <v>180</v>
       </c>
       <c r="N13" t="s">
@@ -1518,7 +1532,7 @@
       <c r="E14" t="s">
         <v>58</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="1" t="s">
         <v>38</v>
       </c>
       <c r="G14" t="s">
@@ -1527,10 +1541,10 @@
       <c r="H14" t="s">
         <v>115</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="1" t="s">
         <v>109</v>
       </c>
       <c r="L14" t="s">
@@ -1547,7 +1561,7 @@
       <c r="E15" t="s">
         <v>59</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G15" t="s">
@@ -1556,10 +1570,10 @@
       <c r="H15" t="s">
         <v>116</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="1" t="s">
         <v>165</v>
       </c>
       <c r="L15" t="s">
@@ -1567,45 +1581,45 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="1" t="s">
         <v>82</v>
       </c>
       <c r="H16" t="s">
         <v>117</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="1" t="s">
         <v>132</v>
       </c>
       <c r="K16" t="s">
         <v>110</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="1" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="17" spans="4:12">
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" s="1" t="s">
         <v>184</v>
       </c>
     </row>
@@ -1616,10 +1630,10 @@
       <c r="G18" t="s">
         <v>84</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18" s="1" t="s">
         <v>167</v>
       </c>
       <c r="L18" t="s">
@@ -1627,13 +1641,13 @@
       </c>
     </row>
     <row r="19" spans="4:12">
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="1" t="s">
         <v>135</v>
       </c>
       <c r="L19" t="s">
@@ -1641,7 +1655,7 @@
       </c>
     </row>
     <row r="20" spans="4:12">
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>38</v>
       </c>
       <c r="G20" t="s">
@@ -1658,7 +1672,7 @@
       <c r="G21" t="s">
         <v>86</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="1" t="s">
         <v>137</v>
       </c>
     </row>
@@ -1666,7 +1680,7 @@
       <c r="E22" t="s">
         <v>65</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="1" t="s">
         <v>87</v>
       </c>
       <c r="I22" t="s">
@@ -1674,13 +1688,13 @@
       </c>
     </row>
     <row r="23" spans="4:12">
-      <c r="E23" t="s">
+      <c r="E23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G23" t="s">
         <v>88</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="1" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1688,15 +1702,15 @@
       <c r="G24" t="s">
         <v>89</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="1" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="25" spans="4:12">
-      <c r="G25" t="s">
+      <c r="G25" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="1" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1704,20 +1718,20 @@
       <c r="G26" t="s">
         <v>62</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="1" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="27" spans="4:12">
-      <c r="G27" t="s">
+      <c r="G27" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="1" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="28" spans="4:12">
-      <c r="G28" t="s">
+      <c r="G28" s="1" t="s">
         <v>63</v>
       </c>
       <c r="I28" t="s">
@@ -1725,27 +1739,27 @@
       </c>
     </row>
     <row r="29" spans="4:12">
-      <c r="G29" t="s">
+      <c r="G29" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="30" spans="4:12">
-      <c r="G30" t="s">
+      <c r="G30" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="31" spans="4:12">
-      <c r="G31" t="s">
+      <c r="G31" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="32" spans="4:12">
-      <c r="G32" t="s">
+      <c r="G32" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="33" spans="7:7">
-      <c r="G33" t="s">
+      <c r="G33" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1765,7 +1779,7 @@
       </c>
     </row>
     <row r="37" spans="7:7">
-      <c r="G37" t="s">
+      <c r="G37" s="1" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1780,7 +1794,7 @@
       </c>
     </row>
     <row r="40" spans="7:7">
-      <c r="G40" t="s">
+      <c r="G40" s="1" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>